<commit_message>
Adds type material and locality
</commit_message>
<xml_diff>
--- a/templates/CoLDP_flat_schema.xlsx
+++ b/templates/CoLDP_flat_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col+/coldp/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE4335-8427-D041-9514-D11186D1B2E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1783B8-776E-EF46-9996-46DFA86ACB74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24420" windowHeight="13440" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24420" windowHeight="13440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>taxonID</t>
   </si>
@@ -204,6 +204,21 @@
   </si>
   <si>
     <t>extinct</t>
+  </si>
+  <si>
+    <t>cultivarEpithet</t>
+  </si>
+  <si>
+    <t>appendedPhrase</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>typeMaterial</t>
+  </si>
+  <si>
+    <t>typeLocality</t>
   </si>
 </sst>
 </file>
@@ -554,19 +569,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="52" customWidth="1"/>
-    <col min="6" max="1025" width="11.5"/>
+    <col min="1" max="6" width="52" customWidth="1"/>
+    <col min="7" max="1026" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,12 +589,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -636,10 +654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -648,7 +666,7 @@
     <col min="14" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -671,21 +689,36 @@
         <v>14</v>
       </c>
       <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -793,10 +826,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -805,7 +838,7 @@
     <col min="9" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -829,6 +862,9 @@
       </c>
       <c r="H1" t="s">
         <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -843,10 +879,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -855,7 +891,7 @@
     <col min="5" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -866,6 +902,9 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -883,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replace original with originalNameId. Adds Name.uninomial. Add NameUsage excel template. Fix diagrams
</commit_message>
<xml_diff>
--- a/templates/CoLDP_flat_schema.xlsx
+++ b/templates/CoLDP_flat_schema.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col/coldp/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAA883B-D2B6-994B-A4EF-7460630BB22D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDA275-48B9-DA44-9799-82086E78F86A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="13600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="10" r:id="rId1"/>
-    <sheet name="Description" sheetId="1" r:id="rId2"/>
-    <sheet name="Distribution" sheetId="2" r:id="rId3"/>
-    <sheet name="Name" sheetId="3" r:id="rId4"/>
-    <sheet name="NameRel" sheetId="4" r:id="rId5"/>
-    <sheet name="Media" sheetId="5" r:id="rId6"/>
-    <sheet name="Reference" sheetId="6" r:id="rId7"/>
-    <sheet name="Synonym" sheetId="7" r:id="rId8"/>
-    <sheet name="Taxon" sheetId="8" r:id="rId9"/>
-    <sheet name="VernacularName" sheetId="9" r:id="rId10"/>
+    <sheet name="Name" sheetId="3" r:id="rId2"/>
+    <sheet name="NameRelation" sheetId="4" r:id="rId3"/>
+    <sheet name="TypeMaterial" sheetId="11" r:id="rId4"/>
+    <sheet name="Taxon" sheetId="8" r:id="rId5"/>
+    <sheet name="Synonym" sheetId="7" r:id="rId6"/>
+    <sheet name="Distribution" sheetId="2" r:id="rId7"/>
+    <sheet name="Media" sheetId="5" r:id="rId8"/>
+    <sheet name="VernacularName" sheetId="9" r:id="rId9"/>
+    <sheet name="Reference" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>taxonID</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>cultivarEpithet</t>
   </si>
   <si>
-    <t>appendedPhrase</t>
-  </si>
-  <si>
     <t>publishedInID</t>
   </si>
   <si>
@@ -102,21 +96,9 @@
     <t>publishedInYear</t>
   </si>
   <si>
-    <t>original</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
-    <t>typeStatus</t>
-  </si>
-  <si>
-    <t>typeMaterial</t>
-  </si>
-  <si>
-    <t>typeReferenceID</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -168,15 +150,9 @@
     <t>provisional</t>
   </si>
   <si>
-    <t>accordingTo</t>
-  </si>
-  <si>
     <t>accordingToID</t>
   </si>
   <si>
-    <t>accordingToDate</t>
-  </si>
-  <si>
     <t>extinct</t>
   </si>
   <si>
@@ -189,51 +165,6 @@
     <t>lifezone</t>
   </si>
   <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>subgenus</t>
-  </si>
-  <si>
-    <t>subtribe</t>
-  </si>
-  <si>
-    <t>tribe</t>
-  </si>
-  <si>
-    <t>subfamily</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>superfamily</t>
-  </si>
-  <si>
-    <t>suborder</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>subclass</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>subphylum</t>
-  </si>
-  <si>
-    <t>phylum</t>
-  </si>
-  <si>
-    <t>kingdom</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -289,6 +220,45 @@
   </si>
   <si>
     <t>author2</t>
+  </si>
+  <si>
+    <t>uninomial</t>
+  </si>
+  <si>
+    <t>originalNameId</t>
+  </si>
+  <si>
+    <t>collector</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>parentID</t>
+  </si>
+  <si>
+    <t>appendedNamePhrase</t>
+  </si>
+  <si>
+    <t>scrutinizer</t>
+  </si>
+  <si>
+    <t>scrutinizerDate</t>
   </si>
 </sst>
 </file>
@@ -650,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874A1130-FDCD-334E-85AE-CC536E71BEBD}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -662,89 +632,89 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -753,44 +723,49 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="9" width="37" customWidth="1"/>
+    <col min="1" max="9" width="35" customWidth="1"/>
     <col min="10" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -804,40 +779,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="6" width="52" customWidth="1"/>
-    <col min="7" max="1025" width="11.5"/>
+    <col min="1" max="21" width="20.5" customWidth="1"/>
+    <col min="22" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -846,6 +859,221 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="5" width="46.1640625" customWidth="1"/>
+    <col min="6" max="1025" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2BE15F-D6B7-6C48-9315-BCCFFF3FE266}">
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="29" width="25.1640625" customWidth="1"/>
+    <col min="30" max="1025" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="1025" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -864,16 +1092,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -886,137 +1114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="21" width="20.5" customWidth="1"/>
-    <col min="22" max="1025" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="5" width="46.1640625" customWidth="1"/>
-    <col min="6" max="1025" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1035,28 +1133,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1069,202 +1167,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="9" width="35" customWidth="1"/>
-    <col min="10" max="1025" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="1025" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AC1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="29" width="25.1640625" customWidth="1"/>
-    <col min="30" max="1025" width="11.5"/>
+    <col min="1" max="9" width="37" customWidth="1"/>
+    <col min="10" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>45</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" t="s">
-        <v>58</v>
-      </c>
-      <c r="W1" t="s">
-        <v>59</v>
-      </c>
-      <c r="X1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>